<commit_message>
fixed issue with duplicates in input folder
</commit_message>
<xml_diff>
--- a/BM3KXR.xlsx
+++ b/BM3KXR.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ICBC_E-Stamp_Tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PythonProjects\ICBC_E-Stamp_Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F821EEEA-4BF2-4038-BAE6-D85152C4BF76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354EC80C-BB50-4497-B757-B3C3807FD86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -604,7 +604,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:C11"/>
+      <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
add pymupdffonts and icbc logo.ico
</commit_message>
<xml_diff>
--- a/BM3KXR.xlsx
+++ b/BM3KXR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PythonProjects\ICBC_E-Stamp_Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C582ED5F-3F2A-48E4-9974-F76EA9C5532E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D708604-C051-440B-B8DD-C88E10CEA2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20595" yWindow="1380" windowWidth="21600" windowHeight="11205" tabRatio="595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="19" r:id="rId1"/>
@@ -604,7 +604,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
correct typo in excel sheet
</commit_message>
<xml_diff>
--- a/BM3KXR.xlsx
+++ b/BM3KXR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PythonProjects\ICBC_E-Stamp_Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D708604-C051-440B-B8DD-C88E10CEA2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63464D95-D91A-430F-A4DB-B8AAC9F9B3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20595" yWindow="1380" windowWidth="21600" windowHeight="11205" tabRatio="595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="19" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>In Microsoft Edge: edge://settings/downloads</t>
   </si>
   <si>
-    <t>a) Set downloads to "C:\Users&lt;your_username&gt;\Downloads"</t>
-  </si>
-  <si>
     <t>b) Toggle off "Ask me what to do with each download"</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>Broker number:</t>
+  </si>
+  <si>
+    <t>a) Set downloads to "C:\Users\&lt;your_username&gt;\Downloads"</t>
   </si>
 </sst>
 </file>
@@ -604,7 +604,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -658,7 +658,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
@@ -732,7 +732,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="B18" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -742,15 +742,15 @@
     </row>
     <row r="19" spans="1:7">
       <c r="B19" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="17" t="s">
         <v>10</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>11</v>
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
@@ -760,18 +760,18 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
         <v>12</v>
-      </c>
-      <c r="B21" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="17" t="s">
         <v>14</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>15</v>
       </c>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
@@ -781,10 +781,10 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="18" t="s">
         <v>16</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>17</v>
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>

</xml_diff>

<commit_message>
ChatGpt debug fixes issue with renaming pdfs that was fixed in last update but broken again for unknown reason
</commit_message>
<xml_diff>
--- a/BM3KXR.xlsx
+++ b/BM3KXR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PythonProjects\ICBC_E-Stamp_Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63464D95-D91A-430F-A4DB-B8AAC9F9B3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D943118F-F246-48E2-BCFA-DACE8E20CD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24375" yWindow="2955" windowWidth="21600" windowHeight="11205" tabRatio="595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="19" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Customer copy only:</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>a) Set downloads to "C:\Users\&lt;your_username&gt;\Downloads"</t>
+  </si>
+  <si>
+    <t>Output directory:</t>
   </si>
 </sst>
 </file>
@@ -259,7 +262,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -301,6 +304,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -601,10 +607,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{556FC970-1EB5-4487-B0BD-EA9C98D85591}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -634,8 +640,8 @@
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
       <c r="D3" s="9"/>
       <c r="F3" s="9"/>
     </row>
@@ -648,8 +654,8 @@
         <f>CONCATENATE("Agency name (character limit: ", LEN(B5), "/17 ):")</f>
         <v>Agency name (character limit: 0/17 ):</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:7">
@@ -660,8 +666,8 @@
       <c r="A7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
       <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:7">
@@ -671,107 +677,95 @@
       <c r="A9" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
       <c r="D9" s="10"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-    </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1">
-      <c r="A13" s="1" t="s">
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="3"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="19"/>
+    </row>
+    <row r="15" spans="1:7" ht="15" customHeight="1">
+      <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1">
-      <c r="A14" s="21" t="s">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" ht="15" customHeight="1">
+      <c r="A16" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="19" t="str">
+      <c r="B16" s="20" t="str">
         <f>HYPERLINK("https://github.com/WebDevBernard/ICBC_E-Stamp_Tool")</f>
         <v>https://github.com/WebDevBernard/ICBC_E-Stamp_Tool</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="11"/>
-    </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1">
-      <c r="A15" s="22"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-    </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1">
-      <c r="A16" s="22"/>
-      <c r="B16" s="20"/>
       <c r="C16" s="20"/>
       <c r="D16" s="20"/>
+      <c r="E16" s="11"/>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="23"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+    </row>
+    <row r="18" spans="1:7" ht="15" customHeight="1">
+      <c r="A18" s="23"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+    </row>
+    <row r="19" spans="1:7" ht="15" customHeight="1">
+      <c r="A19" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B19" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="B18" s="14" t="s">
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="B20" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="B19" s="16" t="s">
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="B21" s="16" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
@@ -781,37 +775,58 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B25" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="6"/>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="7"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="6"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="8"/>
+      <c r="A28" s="7"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B14:D16"/>
-    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B16:D18"/>
+    <mergeCell ref="A16:A18"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B7:C7"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:C9" xr:uid="{A1C65328-437F-4708-9530-8981183AC5EC}">
       <formula1>"Timestamp, Today"</formula1>
     </dataValidation>

</xml_diff>